<commit_message>
Add start time to timesheet
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
+++ b/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28F3100-1D4F-402E-88D2-8F22FCF275A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA91CF1-7AB5-4A92-9DB4-DA00A340B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1524" windowWidth="17280" windowHeight="9528" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Name:</t>
   </si>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,7 +722,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>0.87847222222222232</v>
+        <v>0.46180555555555564</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1000,13 +1000,19 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="17"/>
+      <c r="A16" s="7">
+        <v>45955</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="17">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D16" s="17"/>
       <c r="E16" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.41666666666666669</v>
       </c>
       <c r="F16" s="13"/>
     </row>

</xml_diff>

<commit_message>
Editted readMe, rm.ed vscode folder, added some documentation
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
+++ b/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7862BC5-E5A7-4F6C-9ED8-8D729471FC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29C047D-FD58-4E5F-B701-E2CC70442496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1524" windowWidth="17280" windowHeight="9528" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Name:</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Began writing report, determined how to integrate ADC into main alongside Fernando, began creating ADC peripheral interface and editted CMakeList.txt to include it after several attempts, tried to create ADC structure to center ADC initialization in one function but failed.</t>
+  </si>
+  <si>
+    <t>Reviewed and editted cleaned up code/ReadMe, adjusted report</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
   <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +728,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>1.1458333333333335</v>
+        <v>1.2041666666666668</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1024,15 +1027,25 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="A17" s="7">
+        <v>45955</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17">
+        <v>0.85138888888888886</v>
+      </c>
+      <c r="D17" s="17">
+        <v>0.90972222222222221</v>
+      </c>
       <c r="E17" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="13"/>
+        <v>5.8333333333333348E-2</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>

</xml_diff>

<commit_message>
Add hours + clean up readme
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
+++ b/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29C047D-FD58-4E5F-B701-E2CC70442496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399B7EAB-6782-4635-A15E-36EDE90BAF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1524" windowWidth="17280" windowHeight="9528" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Name:</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Reviewed and editted cleaned up code/ReadMe, adjusted report</t>
+  </si>
+  <si>
+    <t>Record and edit microprocessor portion of video</t>
+  </si>
+  <si>
+    <t>Clean up readme and edit in frontend portion of video</t>
   </si>
 </sst>
 </file>
@@ -703,7 +709,7 @@
   <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,7 +734,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>1.2041666666666668</v>
+        <v>1.2701388888888892</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1048,26 +1054,46 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="A18" s="7">
+        <v>45956</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="17">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D18" s="17">
+        <v>0.5</v>
+      </c>
       <c r="E18" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="13"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="A19" s="7">
+        <v>45956</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="17">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D19" s="17">
+        <v>0.68402777777777779</v>
+      </c>
       <c r="E19" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="13"/>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>

</xml_diff>

<commit_message>
Update end time for timesheet
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
+++ b/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186B0297-322A-495B-AD5E-1F063CE19D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CA7570-DB6B-40BE-AA8E-9412F9035F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -149,7 +149,7 @@
     <t>Met with group to conduct work; Researched how to use 5V Micro Submersible Mini Water Pump, discovered it needed use of PWM,  configured PWM in main to test it, developed PWM peripheral module to use in main, integrated it into main, added photos, created branch for another sensor</t>
   </si>
   <si>
-    <t>Began researching how Capacitive Soil Moisture Sensor should interface with the microcontroller and the type of data it outputs, started deciding how to modify ADC code to generalize and be used for both photoresitor and this sensor.</t>
+    <t>Began researching how Capacitive Soil Moisture Sensor should interface with the microcontroller and the type of data it outputs, started deciding how to modify ADC code to generalize and be used for both photoresitor and this sensor, made modular way to declare ADC for light or moisture sensor</t>
   </si>
 </sst>
 </file>
@@ -724,7 +724,7 @@
   <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,7 +749,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>1.0347222222222228</v>
+        <v>1.5388888888888892</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1183,10 +1183,12 @@
       <c r="C23" s="17">
         <v>0.47222222222222221</v>
       </c>
-      <c r="D23" s="17"/>
+      <c r="D23" s="17">
+        <v>0.50416666666666665</v>
+      </c>
       <c r="E23" s="10">
         <f t="shared" si="0"/>
-        <v>-0.47222222222222221</v>
+        <v>3.1944444444444442E-2</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Update timesheet to do some quick adjusts
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
+++ b/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CA7570-DB6B-40BE-AA8E-9412F9035F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C0AEA3-508D-4774-8BB3-0E9255CE5F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Name:</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Began researching how Capacitive Soil Moisture Sensor should interface with the microcontroller and the type of data it outputs, started deciding how to modify ADC code to generalize and be used for both photoresitor and this sensor, made modular way to declare ADC for light or moisture sensor</t>
+  </si>
+  <si>
+    <t>Changed file name's of ADC and related dependencies to make the module more generalizable</t>
   </si>
 </sst>
 </file>
@@ -723,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,7 +752,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>1.5388888888888892</v>
+        <v>0.73333333333333361</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1195,15 +1198,23 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="17"/>
+      <c r="A24" s="7">
+        <v>45970</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="17">
+        <v>0.80555555555555558</v>
+      </c>
       <c r="D24" s="17"/>
       <c r="E24" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="13"/>
+        <v>-0.80555555555555558</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>

</xml_diff>

<commit_message>
Adjust end time due to making fix
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
+++ b/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E55FB0-7C17-4139-B427-BB38D421E14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC68C81E-A0BD-471D-9A07-EAC5CDC8BD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -727,7 +727,7 @@
   <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,7 +752,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>1.5493055555555557</v>
+        <v>1.552777777777778</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1208,11 +1208,11 @@
         <v>0.80555555555555558</v>
       </c>
       <c r="D24" s="17">
-        <v>0.81597222222222221</v>
+        <v>0.81944444444444442</v>
       </c>
       <c r="E24" s="10">
         <f t="shared" si="0"/>
-        <v>1.041666666666663E-2</v>
+        <v>1.388888888888884E-2</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
GUYS THE MOTOR WORKS
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
+++ b/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9EC769-B4DA-4962-BD4C-B243E4874B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C97A908-3992-4F64-863E-FE5AA32A4AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Name:</t>
   </si>
@@ -161,7 +161,7 @@
     <t>Got together, started integrating ADC branch and rearranged main to work as desired for prototype, created GPIO for inputs and started investigating interrupt system, created external switch to interface with micro, looked into getting wifi created to flash onto ESP32</t>
   </si>
   <si>
-    <t>Got together with group, beginning doing gpio integration to set up sensor set up</t>
+    <t>Got together with group, started doing gpio integration to set up sensor set up, created prototype board,  connected and tested moisture sensor, connected and tested new photoresistor, created wires for relay and power bank and tested water motor, editted main to reflect prototype behavior</t>
   </si>
 </sst>
 </file>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,7 +761,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>1.3923611111111116</v>
+        <v>2.1243055555555559</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1270,15 +1270,21 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
+      <c r="A27" s="7">
+        <v>45974</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="C27" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D27" s="17"/>
+      <c r="D27" s="17">
+        <v>0.7319444444444444</v>
+      </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>-0.45833333333333331</v>
+        <v>0.27361111111111108</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Accidentally broke build in merge, but it's fixed now I swear
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
+++ b/Documentation/TimeSheets/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C97A908-3992-4F64-863E-FE5AA32A4AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD21E8D1-1594-47EF-8213-2A01C9E7E5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -736,7 +736,7 @@
   <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,7 +761,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>2.1243055555555559</v>
+        <v>2.130555555555556</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1280,11 +1280,11 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D27" s="17">
-        <v>0.7319444444444444</v>
+        <v>0.73819444444444449</v>
       </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>0.27361111111111108</v>
+        <v>0.27986111111111117</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>41</v>

</xml_diff>